<commit_message>
chore: Update Sheet template for duplicate transaction
</commit_message>
<xml_diff>
--- a/resources/Copy of Sample Sheet.xlsx
+++ b/resources/Copy of Sample Sheet.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="41">
   <si>
     <t>Update</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>ABC GAS STATION</t>
   </si>
   <si>
     <t>EmailId</t>
@@ -391,7 +403,17 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
     <dxf>
       <font/>
       <fill>
@@ -636,16 +658,16 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="11.0"/>
-    <col customWidth="1" min="2" max="2" width="23.13"/>
+    <col customWidth="1" min="2" max="2" width="21.88"/>
     <col customWidth="1" min="5" max="5" width="8.75"/>
-    <col customWidth="1" min="6" max="6" width="20.75"/>
+    <col customWidth="1" min="6" max="6" width="18.88"/>
     <col customWidth="1" min="7" max="7" width="11.5"/>
     <col customWidth="1" hidden="1" min="8" max="8" width="23.25"/>
     <col customWidth="1" min="9" max="9" width="23.25"/>
     <col customWidth="1" min="10" max="10" width="29.13"/>
     <col customWidth="1" min="11" max="11" width="11.88"/>
     <col customWidth="1" min="12" max="14" width="4.25"/>
-    <col customWidth="1" min="15" max="15" width="25.38"/>
+    <col customWidth="1" min="15" max="15" width="13.63"/>
     <col customWidth="1" min="16" max="16" width="18.63"/>
   </cols>
   <sheetData>
@@ -844,26 +866,106 @@
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="20"/>
-      <c r="P5" s="23"/>
+      <c r="A5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="6">
+        <v>45635.729467592595</v>
+      </c>
+      <c r="C5" s="7">
+        <v>6.07</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="16">
+        <v>45670.05351851852</v>
+      </c>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
     </row>
     <row r="6">
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="26"/>
-      <c r="P6" s="27"/>
+      <c r="A6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="18">
+        <v>45668.2146875</v>
+      </c>
+      <c r="C6" s="19">
+        <v>-1234.0</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="20"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="23">
+        <v>45682.85207175926</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="25"/>
@@ -14428,11 +14530,16 @@
   </sheetData>
   <conditionalFormatting sqref="A1:P969">
     <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A1="Duplicate"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:P969">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$D1="Debit"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:P969">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$D1="Credit"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14442,8 +14549,12 @@
     <hyperlink r:id="rId3" ref="M3"/>
     <hyperlink r:id="rId4" ref="N3"/>
     <hyperlink r:id="rId5" ref="M4"/>
+    <hyperlink r:id="rId6" ref="M5"/>
+    <hyperlink r:id="rId7" ref="N5"/>
+    <hyperlink r:id="rId8" ref="M6"/>
+    <hyperlink r:id="rId9" ref="N6"/>
   </hyperlinks>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -14498,7 +14609,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>12</v>
@@ -14579,7 +14690,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
@@ -31357,12 +31468,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:P255">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$D1="Debit"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:P255">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$D1="Credit"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>